<commit_message>
add SubTotal for Template outSource
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/Outsourcing Recognising Template.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/Outsourcing Recognising Template.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
   <si>
     <t>Outsourcing Recognising Report</t>
   </si>
@@ -238,9 +238,6 @@
   </si>
   <si>
     <t>{TotalBuy}</t>
-  </si>
-  <si>
-    <t>{TotalBalance}</t>
   </si>
   <si>
     <t>Credit No</t>
@@ -578,6 +575,8 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="14" fillId="7" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -590,8 +589,6 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="7" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -916,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AF18" sqref="AF18"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AJ19" sqref="V10:AJ19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -957,79 +954,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="23.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
-      <c r="U1" s="42"/>
-      <c r="V1" s="42"/>
-      <c r="W1" s="42"/>
-      <c r="X1" s="42"/>
-      <c r="Y1" s="42"/>
-      <c r="Z1" s="42"/>
-      <c r="AA1" s="42"/>
-      <c r="AB1" s="42"/>
-      <c r="AC1" s="42"/>
-      <c r="AD1" s="42"/>
-      <c r="AE1" s="42"/>
-      <c r="AF1" s="42"/>
-      <c r="AG1" s="42"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="44"/>
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="44"/>
     </row>
     <row r="2" spans="1:34" ht="18.75">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="41" t="s">
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="41"/>
-      <c r="U2" s="41"/>
-      <c r="V2" s="41"/>
-      <c r="W2" s="41"/>
-      <c r="X2" s="41"/>
-      <c r="Y2" s="41"/>
-      <c r="Z2" s="41"/>
-      <c r="AA2" s="41"/>
-      <c r="AB2" s="41"/>
-      <c r="AC2" s="41"/>
-      <c r="AD2" s="41"/>
-      <c r="AE2" s="41"/>
-      <c r="AF2" s="41"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="43"/>
+      <c r="W2" s="43"/>
+      <c r="X2" s="43"/>
+      <c r="Y2" s="43"/>
+      <c r="Z2" s="43"/>
+      <c r="AA2" s="43"/>
+      <c r="AB2" s="43"/>
+      <c r="AC2" s="43"/>
+      <c r="AD2" s="43"/>
+      <c r="AE2" s="43"/>
+      <c r="AF2" s="43"/>
       <c r="AG2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1114,7 +1111,7 @@
         <v>13</v>
       </c>
       <c r="AA3" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB3" s="15" t="s">
         <v>15</v>
@@ -1345,56 +1342,57 @@
       <c r="AG6" s="21"/>
     </row>
     <row r="7" spans="1:34" s="31" customFormat="1" ht="15.75">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="44" t="s">
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="O7" s="44" t="s">
+      <c r="O7" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="P7" s="44" t="s">
+      <c r="P7" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="Q7" s="43" t="s">
+      <c r="Q7" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="R7" s="43"/>
-      <c r="S7" s="43"/>
-      <c r="T7" s="43"/>
-      <c r="U7" s="43"/>
-      <c r="V7" s="43"/>
-      <c r="W7" s="43"/>
-      <c r="X7" s="43"/>
-      <c r="Y7" s="43"/>
-      <c r="Z7" s="43"/>
-      <c r="AA7" s="43"/>
-      <c r="AB7" s="43"/>
-      <c r="AC7" s="43"/>
-      <c r="AD7" s="45" t="s">
+      <c r="R7" s="45"/>
+      <c r="S7" s="45"/>
+      <c r="T7" s="45"/>
+      <c r="U7" s="45"/>
+      <c r="V7" s="45"/>
+      <c r="W7" s="45"/>
+      <c r="X7" s="45"/>
+      <c r="Y7" s="45"/>
+      <c r="Z7" s="45"/>
+      <c r="AA7" s="45"/>
+      <c r="AB7" s="45"/>
+      <c r="AC7" s="45"/>
+      <c r="AD7" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="AE7" s="45" t="s">
+      <c r="AE7" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="AF7" s="45" t="s">
+      <c r="AF7" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="AG7" s="45" t="s">
-        <v>68</v>
+      <c r="AG7" s="41">
+        <f>SUM(AG4:AG6)</f>
+        <v>0</v>
       </c>
       <c r="AH7" s="39"/>
     </row>
@@ -1553,9 +1551,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1762,27 +1763,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8487674-49B6-45FC-BF1C-DB22591417F8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF014768-5FF4-4283-957A-3EF30BE5A982}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="26469b81-5639-404a-a4db-d68c46bc65bf"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="41733dd2-07dd-4b83-9c00-dc1590a38c6d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1807,9 +1796,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF014768-5FF4-4283-957A-3EF30BE5A982}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8487674-49B6-45FC-BF1C-DB22591417F8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="26469b81-5639-404a-a4db-d68c46bc65bf"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="41733dd2-07dd-4b83-9c00-dc1590a38c6d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>